<commit_message>
modified problem definition function
</commit_message>
<xml_diff>
--- a/SpeedUp.xlsx
+++ b/SpeedUp.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="zdt6_10000_200" sheetId="1" r:id="rId1"/>
-    <sheet name="zdt6_10000_200_ch" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="zdt6_10000_200_ch" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="45">
   <si>
     <t>MPI Tasks</t>
   </si>
@@ -40,6 +41,129 @@
   </si>
   <si>
     <t>Speedup</t>
+  </si>
+  <si>
+    <t>JobID</t>
+  </si>
+  <si>
+    <t>JobName</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Partition</t>
+  </si>
+  <si>
+    <t>NTasks</t>
+  </si>
+  <si>
+    <t>AllocCPUS</t>
+  </si>
+  <si>
+    <t>NCPUS</t>
+  </si>
+  <si>
+    <t>ReqNodes</t>
+  </si>
+  <si>
+    <t>Elapsed</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>ExitCode</t>
+  </si>
+  <si>
+    <t>SystemCPU</t>
+  </si>
+  <si>
+    <t>TotalCPU</t>
+  </si>
+  <si>
+    <t>------------</t>
+  </si>
+  <si>
+    <t>----------</t>
+  </si>
+  <si>
+    <t>--------</t>
+  </si>
+  <si>
+    <t>nsga_1_1</t>
+  </si>
+  <si>
+    <t>usu-em</t>
+  </si>
+  <si>
+    <t>COMPLETED</t>
+  </si>
+  <si>
+    <t>1687168.bat+</t>
+  </si>
+  <si>
+    <t>batch</t>
+  </si>
+  <si>
+    <t>paralleln+</t>
+  </si>
+  <si>
+    <t>CANCELLED+</t>
+  </si>
+  <si>
+    <t>1687169.bat+</t>
+  </si>
+  <si>
+    <t>CANCELLED</t>
+  </si>
+  <si>
+    <t>1687170.bat+</t>
+  </si>
+  <si>
+    <t>1687173.bat+</t>
+  </si>
+  <si>
+    <t>nsga_1_2</t>
+  </si>
+  <si>
+    <t>1687175.bat+</t>
+  </si>
+  <si>
+    <t>nsga_1_4</t>
+  </si>
+  <si>
+    <t>1687176.bat+</t>
+  </si>
+  <si>
+    <t>nsga_1_8</t>
+  </si>
+  <si>
+    <t>1687178.bat+</t>
+  </si>
+  <si>
+    <t>1687179.bat+</t>
+  </si>
+  <si>
+    <t>nsga_1_16</t>
+  </si>
+  <si>
+    <t>1687180.bat+</t>
+  </si>
+  <si>
+    <t>nsga_1_32</t>
+  </si>
+  <si>
+    <t>1687182.bat+</t>
+  </si>
+  <si>
+    <t>nsga_2_32</t>
+  </si>
+  <si>
+    <t>1687184.bat+</t>
+  </si>
+  <si>
+    <t>1687186.bat+</t>
   </si>
 </sst>
 </file>
@@ -49,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -57,13 +181,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,11 +220,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="47" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="47" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="47" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -145,7 +302,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -231,10 +387,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>zdt6_10000_200!$B$2:$B$15</c:f>
+              <c:f>zdt6_10000_200!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -254,27 +410,24 @@
                   <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64.0</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128.0</c:v>
+                  <c:v>192.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>192.0</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>256.0</c:v>
+                  <c:v>320.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>320.0</c:v>
+                  <c:v>384.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>384.0</c:v>
+                  <c:v>448.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>448.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>512.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -282,51 +435,48 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>zdt6_10000_200!$D$2:$D$15</c:f>
+              <c:f>zdt6_10000_200!$D$2:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.000</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98442454140524</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99432060064244</c:v>
+                  <c:v>0.994047619047619</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.978621898032643</c:v>
+                  <c:v>1.006024096385542</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.957243796065287</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.914487592130573</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.828975184261146</c:v>
+                  <c:v>0.732456140350877</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.65795036852229</c:v>
+                  <c:v>1.464912280701754</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31.31590073704458</c:v>
+                  <c:v>2.929824561403509</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>62.63180147408917</c:v>
+                  <c:v>5.859649122807017</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>125.2636029481783</c:v>
+                  <c:v>11.71929824561404</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>250.5272058963567</c:v>
+                  <c:v>23.43859649122807</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>501.0544117927134</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1002.108823585427</c:v>
+                  <c:v>46.87719298245614</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -341,11 +491,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="967843968"/>
-        <c:axId val="966959440"/>
+        <c:axId val="-110468800"/>
+        <c:axId val="-89627968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="967843968"/>
+        <c:axId val="-110468800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -470,12 +620,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="966959440"/>
+        <c:crossAx val="-89627968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="966959440"/>
+        <c:axId val="-89627968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -532,7 +682,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="967843968"/>
+        <c:crossAx val="-110468800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1136,7 +1286,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="134" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1433,10 +1583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1468,8 +1618,8 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <f>3 + 25.538 /60</f>
-        <v>3.4256333333333333</v>
+        <f>2 + 47 /60</f>
+        <v>2.7833333333333332</v>
       </c>
       <c r="D2" s="1">
         <f>$C$2/C2</f>
@@ -1484,12 +1634,12 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <f>3+28.79 /60</f>
-        <v>3.4798333333333336</v>
+        <f>2+47/60</f>
+        <v>2.7833333333333332</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D15" si="0">$C$2/C3</f>
-        <v>0.98442454140523961</v>
+        <f t="shared" ref="D3:D14" si="0">$C$2/C3</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1500,12 +1650,12 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <f>3+26.712 /60</f>
-        <v>3.4451999999999998</v>
+        <f>2+48/60</f>
+        <v>2.8</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>0.99432060064243977</v>
+        <v>0.99404761904761907</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1516,12 +1666,12 @@
         <v>8</v>
       </c>
       <c r="C5" s="1">
-        <f>3+30.028 /60</f>
-        <v>3.5004666666666666</v>
+        <f>2+46 /60</f>
+        <v>2.7666666666666666</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>0.97862189803264332</v>
+        <v>1.0060240963855422</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1532,12 +1682,12 @@
         <v>16</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C4:C15" si="1">C5/2</f>
-        <v>1.7502333333333333</v>
+        <f>2+47/60</f>
+        <v>2.7833333333333332</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>1.9572437960652866</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1548,151 +1698,1562 @@
         <v>32</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="1"/>
-        <v>0.87511666666666665</v>
+        <f>2+47/60</f>
+        <v>2.7833333333333332</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>3.9144875921305733</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>64</v>
+        <f t="shared" ref="B8:B14" si="1">A8*64</f>
+        <v>128</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="1"/>
-        <v>0.43755833333333333</v>
+        <f>3+48/60</f>
+        <v>3.8</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>7.8289751842611466</v>
+        <v>0.73245614035087725</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9:B15" si="2">A9*64</f>
-        <v>128</v>
+        <f t="shared" si="1"/>
+        <v>192</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="1"/>
-        <v>0.21877916666666666</v>
+        <f t="shared" ref="C9:C14" si="2">C8/2</f>
+        <v>1.9</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>15.657950368522293</v>
+        <v>1.4649122807017545</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+      <c r="C10" s="1">
         <f t="shared" si="2"/>
-        <v>192</v>
-      </c>
-      <c r="C10" s="1">
-        <f t="shared" si="1"/>
-        <v>0.10938958333333333</v>
+        <v>0.95</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>31.315900737044586</v>
+        <v>2.929824561403509</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11">
+        <f t="shared" si="1"/>
+        <v>320</v>
+      </c>
+      <c r="C11" s="1">
         <f t="shared" si="2"/>
-        <v>256</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" si="1"/>
-        <v>5.4694791666666666E-2</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>62.631801474089173</v>
+        <v>5.859649122807018</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12">
+        <f t="shared" si="1"/>
+        <v>384</v>
+      </c>
+      <c r="C12" s="1">
         <f t="shared" si="2"/>
-        <v>320</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" si="1"/>
-        <v>2.7347395833333333E-2</v>
+        <v>0.23749999999999999</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>125.26360294817835</v>
+        <v>11.719298245614036</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13">
+        <f t="shared" si="1"/>
+        <v>448</v>
+      </c>
+      <c r="C13" s="1">
         <f t="shared" si="2"/>
-        <v>384</v>
-      </c>
-      <c r="C13" s="1">
-        <f t="shared" si="1"/>
-        <v>1.3673697916666666E-2</v>
+        <v>0.11874999999999999</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>250.52720589635669</v>
+        <v>23.438596491228072</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14">
+        <f t="shared" si="1"/>
+        <v>512</v>
+      </c>
+      <c r="C14" s="1">
         <f t="shared" si="2"/>
-        <v>448</v>
-      </c>
-      <c r="C14" s="1">
-        <f t="shared" si="1"/>
-        <v>6.8368489583333332E-3</v>
+        <v>5.9374999999999997E-2</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>501.05441179271338</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="2"/>
-        <v>512</v>
-      </c>
-      <c r="C15" s="1">
-        <f t="shared" si="1"/>
-        <v>3.4184244791666666E-3</v>
-      </c>
-      <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>1002.1088235854268</v>
+        <v>46.877192982456144</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1687168</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3">
+        <v>32</v>
+      </c>
+      <c r="F3">
+        <v>32</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2.4074074074074076E-3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>3.1828703703703701E-4</v>
+      </c>
+      <c r="L3" s="4">
+        <v>2.6459027777777778E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <v>32</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2.4074074074074076E-3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>3.0482638888888888E-4</v>
+      </c>
+      <c r="L4" s="4">
+        <v>3.6623842592592589E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1687168</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2.3032407407407407E-3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1.3449074074074072E-5</v>
+      </c>
+      <c r="L5" s="4">
+        <v>2.2796643518518517E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1687169</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>32</v>
+      </c>
+      <c r="F6">
+        <v>32</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.6469907407407405E-2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1.9212962962962965E-5</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1.6455960648148148E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>32</v>
+      </c>
+      <c r="F7">
+        <v>32</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.6481481481481482E-2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1.9212962962962966E-6</v>
+      </c>
+      <c r="L7" s="4">
+        <v>4.9189814814814814E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1687169</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.6469907407407405E-2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1.728009259259259E-5</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1.6451041666666666E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>1687170</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="5">
+        <v>32</v>
+      </c>
+      <c r="F9" s="5">
+        <v>32</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="6">
+        <v>3.3564814814814812E-4</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="K9" s="8">
+        <v>4.560185185185185E-6</v>
+      </c>
+      <c r="L9" s="8">
+        <v>2.9846064814814812E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>32</v>
+      </c>
+      <c r="F10">
+        <v>32</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>3.3564814814814812E-4</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>2.7662037037037038E-6</v>
+      </c>
+      <c r="L10" s="4">
+        <v>6.226851851851853E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>1687170</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="9">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
+        <v>1</v>
+      </c>
+      <c r="H11" s="10">
+        <v>3.1250000000000001E-4</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="12">
+        <v>1.7939814814814814E-6</v>
+      </c>
+      <c r="L11" s="12">
+        <v>2.922222222222222E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1687173</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <v>32</v>
+      </c>
+      <c r="F12">
+        <v>32</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2.4305555555555556E-3</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>7.7893518518518528E-6</v>
+      </c>
+      <c r="L12" s="4">
+        <v>2.3849189814814814E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>32</v>
+      </c>
+      <c r="F13">
+        <v>32</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2.4305555555555556E-3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2.534722222222222E-6</v>
+      </c>
+      <c r="L13" s="4">
+        <v>5.9953703703703695E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="13">
+        <v>1687173</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13">
+        <v>1</v>
+      </c>
+      <c r="H14" s="14">
+        <v>2.3842592592592591E-3</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="15">
+        <v>0</v>
+      </c>
+      <c r="K14" s="16">
+        <v>5.2430555555555558E-6</v>
+      </c>
+      <c r="L14" s="16">
+        <v>2.378912037037037E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1687175</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15">
+        <v>32</v>
+      </c>
+      <c r="F15">
+        <v>32</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>2.4421296296296296E-3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>8.5069444444444455E-6</v>
+      </c>
+      <c r="L15" s="4">
+        <v>2.4227546296296297E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>32</v>
+      </c>
+      <c r="F16">
+        <v>32</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>2.4421296296296296E-3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>2.7199074074074075E-6</v>
+      </c>
+      <c r="L16" s="4">
+        <v>6.1921296296296294E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1687175</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2.4189814814814816E-3</v>
+      </c>
+      <c r="I17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>5.7754629629629631E-6</v>
+      </c>
+      <c r="L17" s="4">
+        <v>2.4165509259259262E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1687176</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18">
+        <v>32</v>
+      </c>
+      <c r="F18">
+        <v>32</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
+        <v>2.4305555555555556E-3</v>
+      </c>
+      <c r="I18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>8.2638888888888884E-6</v>
+      </c>
+      <c r="L18" s="4">
+        <v>2.3984606481481483E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>32</v>
+      </c>
+      <c r="F19">
+        <v>32</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2.4305555555555556E-3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <v>2.5115740740740739E-6</v>
+      </c>
+      <c r="L19" s="4">
+        <v>5.9606481481481485E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1687176</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2.3958333333333336E-3</v>
+      </c>
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <v>5.7407407407407412E-6</v>
+      </c>
+      <c r="L20" s="4">
+        <v>2.3925000000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1687178</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21">
+        <v>32</v>
+      </c>
+      <c r="F21">
+        <v>32</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2.4537037037037036E-3</v>
+      </c>
+      <c r="I21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
+        <v>8.0787037037037029E-6</v>
+      </c>
+      <c r="L21" s="4">
+        <v>2.4367245370370372E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>32</v>
+      </c>
+      <c r="F22">
+        <v>32</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2.4537037037037036E-3</v>
+      </c>
+      <c r="I22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="4">
+        <v>2.3495370370370375E-6</v>
+      </c>
+      <c r="L22" s="4">
+        <v>5.8449074074074068E-6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1687178</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>2.4305555555555556E-3</v>
+      </c>
+      <c r="I23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4">
+        <v>5.7175925925925931E-6</v>
+      </c>
+      <c r="L23" s="4">
+        <v>2.4308796296296296E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1687179</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24">
+        <v>32</v>
+      </c>
+      <c r="F24">
+        <v>32</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1.3194444444444443E-3</v>
+      </c>
+      <c r="I24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4">
+        <v>6.2615740740740748E-6</v>
+      </c>
+      <c r="L24" s="4">
+        <v>1.3052430555555558E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>32</v>
+      </c>
+      <c r="F25">
+        <v>32</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1.3310185185185185E-3</v>
+      </c>
+      <c r="I25" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="3">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="K25" s="4">
+        <v>1.8402777777777778E-6</v>
+      </c>
+      <c r="L25" s="4">
+        <v>4.8958333333333332E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1687179</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <v>16</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1.3078703703703705E-3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="3">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="K26" s="4">
+        <v>4.4212962962962968E-6</v>
+      </c>
+      <c r="L26" s="4">
+        <v>1.3003472222222223E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1687180</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27">
+        <v>32</v>
+      </c>
+      <c r="F27">
+        <v>32</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2">
+        <v>2.488425925925926E-3</v>
+      </c>
+      <c r="I27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0</v>
+      </c>
+      <c r="K27" s="4">
+        <v>7.9629629629629612E-6</v>
+      </c>
+      <c r="L27" s="4">
+        <v>2.4630439814814814E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>32</v>
+      </c>
+      <c r="F28">
+        <v>32</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
+        <v>2.488425925925926E-3</v>
+      </c>
+      <c r="I28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="4">
+        <v>2.6620370370370374E-6</v>
+      </c>
+      <c r="L28" s="4">
+        <v>5.9953703703703695E-6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1687180</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>16</v>
+      </c>
+      <c r="F29">
+        <v>16</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
+        <v>2.4537037037037036E-3</v>
+      </c>
+      <c r="I29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4">
+        <v>5.2893518518518522E-6</v>
+      </c>
+      <c r="L29" s="4">
+        <v>2.4570370370370367E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1687182</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30">
+        <v>32</v>
+      </c>
+      <c r="F30">
+        <v>32</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <v>2.4768518518518516E-3</v>
+      </c>
+      <c r="I30" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0</v>
+      </c>
+      <c r="K30" s="4">
+        <v>8.3449074074074074E-6</v>
+      </c>
+      <c r="L30" s="4">
+        <v>2.4528819444444446E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>32</v>
+      </c>
+      <c r="F31">
+        <v>32</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2">
+        <v>2.4768518518518516E-3</v>
+      </c>
+      <c r="I31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0</v>
+      </c>
+      <c r="K31" s="4">
+        <v>2.6273148148148148E-6</v>
+      </c>
+      <c r="L31" s="4">
+        <v>5.9606481481481485E-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1687182</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>32</v>
+      </c>
+      <c r="F32">
+        <v>32</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" s="2">
+        <v>2.4537037037037036E-3</v>
+      </c>
+      <c r="I32" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4">
+        <v>5.7060185185185186E-6</v>
+      </c>
+      <c r="L32" s="4">
+        <v>2.4469097222222223E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1687184</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33">
+        <v>64</v>
+      </c>
+      <c r="F33">
+        <v>64</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1.2962962962962963E-3</v>
+      </c>
+      <c r="I33" t="s">
+        <v>26</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0</v>
+      </c>
+      <c r="K33" s="4">
+        <v>2.2916666666666666E-6</v>
+      </c>
+      <c r="L33" s="4">
+        <v>5.3935185185185186E-6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>32</v>
+      </c>
+      <c r="F34">
+        <v>32</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34" s="2">
+        <v>1.3078703703703705E-3</v>
+      </c>
+      <c r="I34" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" s="3">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="K34" s="4">
+        <v>1.967592592592593E-6</v>
+      </c>
+      <c r="L34" s="4">
+        <v>4.9768518518518514E-6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1687184</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>64</v>
+      </c>
+      <c r="F35">
+        <v>64</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35" s="2">
+        <v>1.2847222222222223E-3</v>
+      </c>
+      <c r="I35" t="s">
+        <v>28</v>
+      </c>
+      <c r="J35" s="3">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="K35" s="4">
+        <v>3.2407407407407406E-7</v>
+      </c>
+      <c r="L35" s="4">
+        <v>4.1666666666666661E-7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1687186</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36">
+        <v>64</v>
+      </c>
+      <c r="F36">
+        <v>64</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" s="2">
+        <v>2.4652777777777776E-3</v>
+      </c>
+      <c r="I36" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0</v>
+      </c>
+      <c r="K36" s="4">
+        <v>1.5805555555555557E-4</v>
+      </c>
+      <c r="L36" s="4">
+        <v>4.7607870370370373E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>32</v>
+      </c>
+      <c r="F37">
+        <v>32</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" s="2">
+        <v>2.4652777777777776E-3</v>
+      </c>
+      <c r="I37" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0</v>
+      </c>
+      <c r="K37" s="4">
+        <v>3.7268518518518523E-6</v>
+      </c>
+      <c r="L37" s="4">
+        <v>7.3263888888888893E-6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>